<commit_message>
feat: Update phpoffice/phpspreadsheet to ^5.1
Updated the phpoffice/phpspreadsheet dependency to version 5.1 and made the necessary code changes to ensure compatibility. Also updated the PHP requirement to ^8.0 and removed the roave/security-advisories package.
</commit_message>
<xml_diff>
--- a/samples/10_images/exported_file.xlsx
+++ b/samples/10_images/exported_file.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
-    <t>Date: 02-10-2019 - Department: Sales department</t>
+    <t>Date: 06-01-2026 - Department: Sales department</t>
   </si>
   <si>
     <t>Report by hours:</t>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
   <fonts count="2">
     <font>
@@ -49,6 +49,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="204"/>
     </font>
     <font>
       <b val="1"/>
@@ -56,22 +57,18 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="14"/>
-      <color rgb="FF3B3B38"/>
+      <color rgb="FF4B462A"/>
       <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,13 +78,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD8D8D8"/>
+        <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -101,28 +104,23 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -575,11 +573,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C11" sqref="C11"/>
@@ -589,11 +587,11 @@
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="true" style="0"/>
     <col min="2" max="2" width="24.7109375" customWidth="true" style="0"/>
-    <col min="19" max="19" width="25.28515625" customWidth="true" style="0"/>
     <col min="3" max="3" width="24.7109375" customWidth="true" style="0"/>
     <col min="4" max="4" width="24.7109375" customWidth="true" style="0"/>
     <col min="5" max="5" width="24.7109375" customWidth="true" style="0"/>
     <col min="6" max="6" width="24.7109375" customWidth="true" style="0"/>
+    <col min="19" max="19" width="25.28515625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
@@ -680,21 +678,13 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells>
     <mergeCell ref="A2:T2"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>